<commit_message>
started analysis, read in data, outline
</commit_message>
<xml_diff>
--- a/Oct Likert Numbers.xlsx
+++ b/Oct Likert Numbers.xlsx
@@ -1,18 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11108"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Stelara Study\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peterhiggins/Documents/RCode/elena_skin_uste/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F4D813B-7D50-7F49-8487-74C6DB01C8BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6500"/>
+    <workbookView xWindow="21860" yWindow="1680" windowWidth="30580" windowHeight="27720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="path" sheetId="3" r:id="rId1"/>
+    <sheet name="endo" sheetId="4" r:id="rId2"/>
+    <sheet name="imaging" sheetId="2" r:id="rId3"/>
+    <sheet name="alt_format" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="29">
   <si>
     <t>PATH</t>
   </si>
@@ -40,12 +44,424 @@
   <si>
     <t>IMAGING</t>
   </si>
+  <si>
+    <t>mrn</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>endo_likert</t>
+  </si>
+  <si>
+    <t>path_likert</t>
+  </si>
+  <si>
+    <t>imaging_likert</t>
+  </si>
+  <si>
+    <t>A likert score includes 5 evaluation endpoints:</t>
+  </si>
+  <si>
+    <r>
+      <t>(1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>significantly worse</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>(2)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>slightly worse</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>(3)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>no change</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>(4)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>slightly better</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>(5)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>completely better</t>
+    </r>
+  </si>
+  <si>
+    <t>For the sake of this evaluation:</t>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Severe disease to no disease = 5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>No disease to severe disease = 1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Mild disease to no disease = 4 (slightly better)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>No disease to mild disease = 2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Mild ileal to mild colonic disease = 3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Moderate ileal to moderate colonic disease = 3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Severe ileal to severe colonic disease = 3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Mild colonic to mild ileal disease = 3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Moderate colonic to moderate ileal disease = 3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Severe colonic to severe ileal disease = 3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Severe ulceration &gt;ulceration &gt;apthous&gt; inflammation (unless described as worse)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Large extent moderate disease&gt;single big ulcer</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -58,6 +474,24 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Symbol"/>
+      <charset val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -80,7 +514,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -95,6 +529,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -375,25 +818,2820 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K97"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0910C56-8B49-D448-AA25-BA8CD6F27753}">
+  <dimension ref="A1:C93"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2" s="3">
+        <v>17663550</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3" s="3">
+        <v>100238954</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4" s="3">
+        <v>32647807</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5" s="3">
+        <v>29423933</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A6" s="3">
+        <v>26166548</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A7" s="3">
+        <v>40222303</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A8" s="3">
+        <v>10982649</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A9" s="3">
+        <v>22327689</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A10" s="3">
+        <v>100412990</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A11" s="3">
+        <v>31683831</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A12" s="3">
+        <v>25476153</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A13" s="3">
+        <v>38235461</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A14" s="3">
+        <v>41928037</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A15" s="3">
+        <v>100237579</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A16" s="3">
+        <v>15332992</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A17" s="3">
+        <v>24990552</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A18" s="3">
+        <v>100202389</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A19" s="3">
+        <v>100305305</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A20" s="3">
+        <v>100260630</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A21" s="3">
+        <v>32437412</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A22" s="3">
+        <v>100373506</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A23" s="3">
+        <v>34560471</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A24" s="3">
+        <v>100832303</v>
+      </c>
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A25" s="3">
+        <v>14348505</v>
+      </c>
+      <c r="B25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A26" s="3">
+        <v>39636505</v>
+      </c>
+      <c r="B26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A27" s="3">
+        <v>23419919</v>
+      </c>
+      <c r="B27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A28" s="3">
+        <v>100673966</v>
+      </c>
+      <c r="B28" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A29" s="3">
+        <v>38339621</v>
+      </c>
+      <c r="B29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A30" s="3">
+        <v>100765596</v>
+      </c>
+      <c r="B30" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A31" s="3">
+        <v>37535758</v>
+      </c>
+      <c r="B31" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A32" s="3">
+        <v>100486962</v>
+      </c>
+      <c r="B32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A33" s="3">
+        <v>100291718</v>
+      </c>
+      <c r="B33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A34" s="3">
+        <v>100876283</v>
+      </c>
+      <c r="B34" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A35" s="3">
+        <v>38619585</v>
+      </c>
+      <c r="B35" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A36" s="3">
+        <v>100186919</v>
+      </c>
+      <c r="B36" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A37" s="3">
+        <v>100166941</v>
+      </c>
+      <c r="B37" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A38" s="3">
+        <v>23033781</v>
+      </c>
+      <c r="B38" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A39" s="3">
+        <v>16946862</v>
+      </c>
+      <c r="B39" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A40" s="3">
+        <v>100347819</v>
+      </c>
+      <c r="B40" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A41" s="3">
+        <v>41925437</v>
+      </c>
+      <c r="B41" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A42" s="3">
+        <v>16894321</v>
+      </c>
+      <c r="B42" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A43" s="3">
+        <v>100490151</v>
+      </c>
+      <c r="B43" t="s">
+        <v>2</v>
+      </c>
+      <c r="C43" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A44" s="3">
+        <v>32917707</v>
+      </c>
+      <c r="B44" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A45" s="3">
+        <v>40353379</v>
+      </c>
+      <c r="B45" t="s">
+        <v>2</v>
+      </c>
+      <c r="C45" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A46" s="3">
+        <v>100054442</v>
+      </c>
+      <c r="B46" t="s">
+        <v>2</v>
+      </c>
+      <c r="C46" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A47" s="3">
+        <v>100081485</v>
+      </c>
+      <c r="B47" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A48" s="3">
+        <v>24956684</v>
+      </c>
+      <c r="B48" t="s">
+        <v>2</v>
+      </c>
+      <c r="C48" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A49" s="3">
+        <v>19245524</v>
+      </c>
+      <c r="B49" t="s">
+        <v>2</v>
+      </c>
+      <c r="C49" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A50" s="3">
+        <v>100746009</v>
+      </c>
+      <c r="B50" t="s">
+        <v>2</v>
+      </c>
+      <c r="C50" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A51" s="3">
+        <v>41648946</v>
+      </c>
+      <c r="B51" t="s">
+        <v>2</v>
+      </c>
+      <c r="C51" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A52" s="3">
+        <v>41515235</v>
+      </c>
+      <c r="B52" t="s">
+        <v>2</v>
+      </c>
+      <c r="C52" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A53" s="3">
+        <v>13758645</v>
+      </c>
+      <c r="B53" t="s">
+        <v>2</v>
+      </c>
+      <c r="C53" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A54" s="3">
+        <v>32951624</v>
+      </c>
+      <c r="B54" t="s">
+        <v>2</v>
+      </c>
+      <c r="C54" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A55" s="3">
+        <v>36494463</v>
+      </c>
+      <c r="B55" t="s">
+        <v>2</v>
+      </c>
+      <c r="C55" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A56" s="3">
+        <v>100543977</v>
+      </c>
+      <c r="B56" t="s">
+        <v>2</v>
+      </c>
+      <c r="C56" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A57" s="3">
+        <v>100509202</v>
+      </c>
+      <c r="B57" t="s">
+        <v>2</v>
+      </c>
+      <c r="C57" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A58" s="3">
+        <v>100458631</v>
+      </c>
+      <c r="B58" t="s">
+        <v>2</v>
+      </c>
+      <c r="C58" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A59" s="3">
+        <v>27493518</v>
+      </c>
+      <c r="B59" t="s">
+        <v>2</v>
+      </c>
+      <c r="C59" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A60" s="3">
+        <v>32318423</v>
+      </c>
+      <c r="B60" t="s">
+        <v>2</v>
+      </c>
+      <c r="C60" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A61" s="3">
+        <v>21741358</v>
+      </c>
+      <c r="B61" t="s">
+        <v>2</v>
+      </c>
+      <c r="C61" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A62" s="3">
+        <v>23316468</v>
+      </c>
+      <c r="B62" t="s">
+        <v>2</v>
+      </c>
+      <c r="C62" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A63" s="3">
+        <v>100617086</v>
+      </c>
+      <c r="B63" t="s">
+        <v>2</v>
+      </c>
+      <c r="C63" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A64" s="3">
+        <v>100041859</v>
+      </c>
+      <c r="B64" t="s">
+        <v>2</v>
+      </c>
+      <c r="C64" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A65" s="3">
+        <v>41480661</v>
+      </c>
+      <c r="B65" t="s">
+        <v>2</v>
+      </c>
+      <c r="C65" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A66" s="3">
+        <v>36478834</v>
+      </c>
+      <c r="B66" t="s">
+        <v>2</v>
+      </c>
+      <c r="C66" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A67" s="3">
+        <v>27502593</v>
+      </c>
+      <c r="B67" t="s">
+        <v>2</v>
+      </c>
+      <c r="C67" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A68" s="3">
+        <v>100061317</v>
+      </c>
+      <c r="B68" t="s">
+        <v>2</v>
+      </c>
+      <c r="C68" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A69" s="3">
+        <v>36558994</v>
+      </c>
+      <c r="B69" t="s">
+        <v>2</v>
+      </c>
+      <c r="C69" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A70" s="3">
+        <v>100491624</v>
+      </c>
+      <c r="B70" t="s">
+        <v>2</v>
+      </c>
+      <c r="C70" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A71" s="3">
+        <v>100898699</v>
+      </c>
+      <c r="B71" t="s">
+        <v>2</v>
+      </c>
+      <c r="C71" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A72" s="3">
+        <v>35042088</v>
+      </c>
+      <c r="B72" t="s">
+        <v>2</v>
+      </c>
+      <c r="C72" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A73" s="3">
+        <v>100280479</v>
+      </c>
+      <c r="B73" t="s">
+        <v>2</v>
+      </c>
+      <c r="C73" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A74" s="3">
+        <v>28764571</v>
+      </c>
+      <c r="B74" t="s">
+        <v>2</v>
+      </c>
+      <c r="C74" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A75" s="3">
+        <v>100546896</v>
+      </c>
+      <c r="B75" t="s">
+        <v>2</v>
+      </c>
+      <c r="C75" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A76" s="3">
+        <v>100222157</v>
+      </c>
+      <c r="B76" t="s">
+        <v>2</v>
+      </c>
+      <c r="C76" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A77" s="3">
+        <v>35353914</v>
+      </c>
+      <c r="B77" t="s">
+        <v>2</v>
+      </c>
+      <c r="C77" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A78" s="3">
+        <v>100157550</v>
+      </c>
+      <c r="B78" t="s">
+        <v>2</v>
+      </c>
+      <c r="C78" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A79" s="3">
+        <v>30883184</v>
+      </c>
+      <c r="B79" t="s">
+        <v>2</v>
+      </c>
+      <c r="C79" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A80" s="3">
+        <v>34074801</v>
+      </c>
+      <c r="B80" t="s">
+        <v>2</v>
+      </c>
+      <c r="C80" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A81" s="3">
+        <v>100041018</v>
+      </c>
+      <c r="B81" t="s">
+        <v>2</v>
+      </c>
+      <c r="C81" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A82" s="3">
+        <v>39205427</v>
+      </c>
+      <c r="B82" t="s">
+        <v>2</v>
+      </c>
+      <c r="C82" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A83" s="3">
+        <v>100738919</v>
+      </c>
+      <c r="B83" t="s">
+        <v>2</v>
+      </c>
+      <c r="C83" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A84" s="3">
+        <v>100728540</v>
+      </c>
+      <c r="B84" t="s">
+        <v>2</v>
+      </c>
+      <c r="C84" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A85" s="3">
+        <v>40858453</v>
+      </c>
+      <c r="B85" t="s">
+        <v>2</v>
+      </c>
+      <c r="C85" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A86" s="3">
+        <v>100008638</v>
+      </c>
+      <c r="B86" t="s">
+        <v>2</v>
+      </c>
+      <c r="C86" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A87" s="3">
+        <v>100378248</v>
+      </c>
+      <c r="B87" t="s">
+        <v>2</v>
+      </c>
+      <c r="C87" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A88" s="3">
+        <v>28859922</v>
+      </c>
+      <c r="B88" t="s">
+        <v>2</v>
+      </c>
+      <c r="C88" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A89" s="3">
+        <v>100067667</v>
+      </c>
+      <c r="B89" t="s">
+        <v>2</v>
+      </c>
+      <c r="C89" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A90" s="3">
+        <v>100296221</v>
+      </c>
+      <c r="B90" t="s">
+        <v>2</v>
+      </c>
+      <c r="C90" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A91" s="3">
+        <v>25185638</v>
+      </c>
+      <c r="B91" t="s">
+        <v>2</v>
+      </c>
+      <c r="C91" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A92" s="3">
+        <v>101012485</v>
+      </c>
+      <c r="B92" t="s">
+        <v>2</v>
+      </c>
+      <c r="C92" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A93" s="3">
+        <v>100300947</v>
+      </c>
+      <c r="B93" t="s">
+        <v>2</v>
+      </c>
+      <c r="C93" s="3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FBD5294-B435-9A45-AF0D-13D44440B011}">
+  <dimension ref="A1:C95"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:XFD24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2" s="3">
+        <v>17663550</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3" s="3">
+        <v>100238954</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4" s="3">
+        <v>32647807</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5" s="3">
+        <v>29423933</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A6" s="3">
+        <v>26166548</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A7" s="3">
+        <v>40222303</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A8" s="3">
+        <v>10982649</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A9" s="3">
+        <v>22327689</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A10" s="3">
+        <v>100412990</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A11" s="3">
+        <v>31683831</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A12" s="3">
+        <v>25476153</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A13" s="3">
+        <v>38235461</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A14" s="3">
+        <v>41928037</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A15" s="3">
+        <v>100237579</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A16" s="3">
+        <v>15332992</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A17" s="3">
+        <v>24990552</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A18" s="3">
+        <v>100202389</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A19" s="3">
+        <v>100305305</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A20" s="3">
+        <v>100260630</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A21" s="3">
+        <v>32437412</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A22" s="3">
+        <v>100373506</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A23" s="3">
+        <v>34560471</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A24" s="3">
+        <v>100448767</v>
+      </c>
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A25" s="3">
+        <v>21682381</v>
+      </c>
+      <c r="B25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A26" s="3">
+        <v>100832303</v>
+      </c>
+      <c r="B26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A27" s="3">
+        <v>14348505</v>
+      </c>
+      <c r="B27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A28" s="3">
+        <v>39636505</v>
+      </c>
+      <c r="B28" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A29" s="3">
+        <v>23419919</v>
+      </c>
+      <c r="B29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A30" s="3">
+        <v>100673966</v>
+      </c>
+      <c r="B30" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A31" s="3">
+        <v>38339621</v>
+      </c>
+      <c r="B31" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A32" s="3">
+        <v>100765596</v>
+      </c>
+      <c r="B32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A33" s="3">
+        <v>37535758</v>
+      </c>
+      <c r="B33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A34" s="3">
+        <v>100486962</v>
+      </c>
+      <c r="B34" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A35" s="3">
+        <v>100291718</v>
+      </c>
+      <c r="B35" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A36" s="3">
+        <v>100876283</v>
+      </c>
+      <c r="B36" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A37" s="3">
+        <v>38619585</v>
+      </c>
+      <c r="B37" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A38" s="3">
+        <v>100186919</v>
+      </c>
+      <c r="B38" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A39" s="3">
+        <v>100166941</v>
+      </c>
+      <c r="B39" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A40" s="3">
+        <v>23033781</v>
+      </c>
+      <c r="B40" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A41" s="3">
+        <v>16946862</v>
+      </c>
+      <c r="B41" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A42" s="3">
+        <v>100347819</v>
+      </c>
+      <c r="B42" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A43" s="3">
+        <v>41925437</v>
+      </c>
+      <c r="B43" t="s">
+        <v>2</v>
+      </c>
+      <c r="C43" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A44" s="3">
+        <v>16894321</v>
+      </c>
+      <c r="B44" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A45" s="3">
+        <v>100490151</v>
+      </c>
+      <c r="B45" t="s">
+        <v>2</v>
+      </c>
+      <c r="C45" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A46" s="3">
+        <v>32917707</v>
+      </c>
+      <c r="B46" t="s">
+        <v>2</v>
+      </c>
+      <c r="C46" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A47" s="3">
+        <v>40353379</v>
+      </c>
+      <c r="B47" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A48" s="3">
+        <v>100054442</v>
+      </c>
+      <c r="B48" t="s">
+        <v>2</v>
+      </c>
+      <c r="C48" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A49" s="3">
+        <v>100081485</v>
+      </c>
+      <c r="B49" t="s">
+        <v>2</v>
+      </c>
+      <c r="C49" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A50" s="3">
+        <v>24956684</v>
+      </c>
+      <c r="B50" t="s">
+        <v>2</v>
+      </c>
+      <c r="C50" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A51" s="3">
+        <v>19245524</v>
+      </c>
+      <c r="B51" t="s">
+        <v>2</v>
+      </c>
+      <c r="C51" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A52" s="3">
+        <v>100746009</v>
+      </c>
+      <c r="B52" t="s">
+        <v>2</v>
+      </c>
+      <c r="C52" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A53" s="3">
+        <v>41648946</v>
+      </c>
+      <c r="B53" t="s">
+        <v>2</v>
+      </c>
+      <c r="C53" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A54" s="3">
+        <v>13758645</v>
+      </c>
+      <c r="B54" t="s">
+        <v>2</v>
+      </c>
+      <c r="C54" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A55" s="3">
+        <v>32951624</v>
+      </c>
+      <c r="B55" t="s">
+        <v>2</v>
+      </c>
+      <c r="C55" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A56" s="3">
+        <v>36494463</v>
+      </c>
+      <c r="B56" t="s">
+        <v>2</v>
+      </c>
+      <c r="C56" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A57" s="3">
+        <v>100543977</v>
+      </c>
+      <c r="B57" t="s">
+        <v>2</v>
+      </c>
+      <c r="C57" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A58" s="3">
+        <v>100509202</v>
+      </c>
+      <c r="B58" t="s">
+        <v>2</v>
+      </c>
+      <c r="C58" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A59" s="3">
+        <v>100458631</v>
+      </c>
+      <c r="B59" t="s">
+        <v>2</v>
+      </c>
+      <c r="C59" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A60" s="3">
+        <v>27493518</v>
+      </c>
+      <c r="B60" t="s">
+        <v>2</v>
+      </c>
+      <c r="C60" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A61" s="3">
+        <v>32318423</v>
+      </c>
+      <c r="B61" t="s">
+        <v>2</v>
+      </c>
+      <c r="C61" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A62" s="3">
+        <v>21741358</v>
+      </c>
+      <c r="B62" t="s">
+        <v>2</v>
+      </c>
+      <c r="C62" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A63" s="3">
+        <v>23316468</v>
+      </c>
+      <c r="B63" t="s">
+        <v>2</v>
+      </c>
+      <c r="C63" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A64" s="3">
+        <v>100617086</v>
+      </c>
+      <c r="B64" t="s">
+        <v>2</v>
+      </c>
+      <c r="C64" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A65" s="3">
+        <v>41480661</v>
+      </c>
+      <c r="B65" t="s">
+        <v>2</v>
+      </c>
+      <c r="C65" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A66" s="3">
+        <v>100041859</v>
+      </c>
+      <c r="B66" t="s">
+        <v>2</v>
+      </c>
+      <c r="C66" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A67" s="3">
+        <v>36478834</v>
+      </c>
+      <c r="B67" t="s">
+        <v>2</v>
+      </c>
+      <c r="C67" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A68" s="3">
+        <v>27502593</v>
+      </c>
+      <c r="B68" t="s">
+        <v>2</v>
+      </c>
+      <c r="C68" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A69" s="3">
+        <v>100061317</v>
+      </c>
+      <c r="B69" t="s">
+        <v>2</v>
+      </c>
+      <c r="C69" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A70" s="3">
+        <v>36558994</v>
+      </c>
+      <c r="B70" t="s">
+        <v>2</v>
+      </c>
+      <c r="C70" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A71" s="3">
+        <v>100491624</v>
+      </c>
+      <c r="B71" t="s">
+        <v>2</v>
+      </c>
+      <c r="C71" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A72" s="3">
+        <v>100898699</v>
+      </c>
+      <c r="B72" t="s">
+        <v>2</v>
+      </c>
+      <c r="C72" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A73" s="3">
+        <v>35042088</v>
+      </c>
+      <c r="B73" t="s">
+        <v>2</v>
+      </c>
+      <c r="C73" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A74" s="3">
+        <v>100280479</v>
+      </c>
+      <c r="B74" t="s">
+        <v>2</v>
+      </c>
+      <c r="C74" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A75" s="3">
+        <v>28764571</v>
+      </c>
+      <c r="B75" t="s">
+        <v>2</v>
+      </c>
+      <c r="C75" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A76" s="3">
+        <v>100546896</v>
+      </c>
+      <c r="B76" t="s">
+        <v>2</v>
+      </c>
+      <c r="C76" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A77" s="3">
+        <v>100222157</v>
+      </c>
+      <c r="B77" t="s">
+        <v>2</v>
+      </c>
+      <c r="C77" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A78" s="3">
+        <v>35353914</v>
+      </c>
+      <c r="B78" t="s">
+        <v>2</v>
+      </c>
+      <c r="C78" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A79" s="3">
+        <v>100157550</v>
+      </c>
+      <c r="B79" t="s">
+        <v>2</v>
+      </c>
+      <c r="C79" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A80" s="3">
+        <v>30883184</v>
+      </c>
+      <c r="B80" t="s">
+        <v>2</v>
+      </c>
+      <c r="C80" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A81" s="3">
+        <v>24474380</v>
+      </c>
+      <c r="B81" t="s">
+        <v>2</v>
+      </c>
+      <c r="C81" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A82" s="3">
+        <v>34074801</v>
+      </c>
+      <c r="B82" t="s">
+        <v>2</v>
+      </c>
+      <c r="C82" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A83" s="3">
+        <v>100041018</v>
+      </c>
+      <c r="B83" t="s">
+        <v>2</v>
+      </c>
+      <c r="C83" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A84" s="3">
+        <v>17851330</v>
+      </c>
+      <c r="B84" t="s">
+        <v>2</v>
+      </c>
+      <c r="C84" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A85" s="3">
+        <v>39205427</v>
+      </c>
+      <c r="B85" t="s">
+        <v>2</v>
+      </c>
+      <c r="C85" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A86" s="3">
+        <v>100728540</v>
+      </c>
+      <c r="B86" t="s">
+        <v>2</v>
+      </c>
+      <c r="C86" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A87" s="3">
+        <v>40858453</v>
+      </c>
+      <c r="B87" t="s">
+        <v>2</v>
+      </c>
+      <c r="C87" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A88" s="3">
+        <v>100008638</v>
+      </c>
+      <c r="B88" t="s">
+        <v>2</v>
+      </c>
+      <c r="C88" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A89" s="3">
+        <v>100378248</v>
+      </c>
+      <c r="B89" t="s">
+        <v>2</v>
+      </c>
+      <c r="C89" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A90" s="3">
+        <v>28859922</v>
+      </c>
+      <c r="B90" t="s">
+        <v>2</v>
+      </c>
+      <c r="C90" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A91" s="3">
+        <v>100067667</v>
+      </c>
+      <c r="B91" t="s">
+        <v>2</v>
+      </c>
+      <c r="C91" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A92" s="3">
+        <v>100296221</v>
+      </c>
+      <c r="B92" t="s">
+        <v>2</v>
+      </c>
+      <c r="C92" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A93" s="3">
+        <v>25185638</v>
+      </c>
+      <c r="B93" t="s">
+        <v>2</v>
+      </c>
+      <c r="C93" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A94" s="3">
+        <v>101012485</v>
+      </c>
+      <c r="B94" t="s">
+        <v>2</v>
+      </c>
+      <c r="C94" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A95" s="3">
+        <v>100300947</v>
+      </c>
+      <c r="B95" t="s">
+        <v>2</v>
+      </c>
+      <c r="C95" s="3">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ED16487-5540-B14F-B20B-5BFD11FAA137}">
+  <dimension ref="A1:C62"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A2" s="3">
+        <v>18414351</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A3" s="3">
+        <v>100637963</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A4" s="3">
+        <v>39991998</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A5" s="3">
+        <v>100238954</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A6" s="3">
+        <v>100387262</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A7" s="3">
+        <v>32647807</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A8" s="3">
+        <v>100581887</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A9" s="3">
+        <v>29299249</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A10" s="3">
+        <v>38235461</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A11" s="3">
+        <v>22916774</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A12" s="3">
+        <v>100260630</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A13" s="3">
+        <v>100035862</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A14" s="3">
+        <v>32437412</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A15" s="3">
+        <v>100373506</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A16" s="3">
+        <v>100806129</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A17" s="3">
+        <v>100448767</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A18" s="3">
+        <v>21682381</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A19" s="3">
+        <v>36558313</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A20" s="3">
+        <v>34422436</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A21" s="3">
+        <v>39636505</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A22" s="3">
+        <v>100451297</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A23" s="3">
+        <v>101135836</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A24" s="3">
+        <v>38553033</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A25" s="3">
+        <v>32286902</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A26" s="3">
+        <v>38910024</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A27" s="3">
+        <v>23033781</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A28" s="3">
+        <v>16946862</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A29" s="3">
+        <v>30129453</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A30" s="3">
+        <v>16894321</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A31" s="3">
+        <v>24082571</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A32" s="3">
+        <v>100081485</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A33" s="3">
+        <v>41515235</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A34" s="3">
+        <v>100532844</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A35" s="3">
+        <v>100608146</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A36" s="3">
+        <v>40425214</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A37" s="3">
+        <v>36494463</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A38" s="3">
+        <v>100244233</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A39" s="3">
+        <v>100543977</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A40" s="3">
+        <v>100356683</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A41" s="3">
+        <v>100205315</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A42" s="3">
+        <v>100913836</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A43" s="3">
+        <v>27493518</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C43" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A44" s="3">
+        <v>15739897</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A45" s="3">
+        <v>23316468</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C45" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A46" s="3">
+        <v>100085703</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C46" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A47" s="3">
+        <v>100777135</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A48" s="3">
+        <v>100070451</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C48" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A49" s="3">
+        <v>23378188</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C49" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A50" s="3">
+        <v>35353914</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C50" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A51" s="3">
+        <v>32250063</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C51" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A52" s="3">
+        <v>100889691</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C52" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A53" s="3">
+        <v>100571124</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C53" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A54" s="3">
+        <v>100199442</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C54" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A55" s="3">
+        <v>100776984</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C55" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A56" s="3">
+        <v>26094331</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C56" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A57" s="3">
+        <v>100399183</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C57" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A58" s="3">
+        <v>25185638</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C58" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A59" s="3">
+        <v>17018449</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C59" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A60" s="3">
+        <v>19021415</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C60" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A61" s="3">
+        <v>23344491</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C61" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A62" s="3">
+        <v>15307456</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C62" s="3">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M60" sqref="M60"/>
+      <selection activeCell="T27" sqref="T27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.6640625" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="3.75" customWidth="1"/>
+    <col min="3" max="3" width="3.6640625" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" customWidth="1"/>
     <col min="7" max="7" width="4.6640625" customWidth="1"/>
-    <col min="9" max="9" width="10.25" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -407,12 +3645,12 @@
       </c>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="15" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>17663550</v>
       </c>
@@ -441,7 +3679,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="15" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>100238954</v>
       </c>
@@ -469,8 +3707,11 @@
       <c r="K4" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O4" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="15" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>32647807</v>
       </c>
@@ -498,8 +3739,11 @@
       <c r="K5" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O5" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>29423933</v>
       </c>
@@ -527,8 +3771,11 @@
       <c r="K6" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O6" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="15" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>26166548</v>
       </c>
@@ -556,8 +3803,11 @@
       <c r="K7" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O7" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="15" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>40222303</v>
       </c>
@@ -585,8 +3835,11 @@
       <c r="K8" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O8" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="15" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>10982649</v>
       </c>
@@ -614,8 +3867,11 @@
       <c r="K9" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O9" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="15" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>22327689</v>
       </c>
@@ -643,8 +3899,11 @@
       <c r="K10" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O10" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="15" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>100412990</v>
       </c>
@@ -672,8 +3931,11 @@
       <c r="K11" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O11" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="15" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>31683831</v>
       </c>
@@ -701,8 +3963,11 @@
       <c r="K12" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O12" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="15" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
         <v>25476153</v>
       </c>
@@ -730,8 +3995,11 @@
       <c r="K13" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O13" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="15" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
         <v>38235461</v>
       </c>
@@ -759,8 +4027,11 @@
       <c r="K14" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O14" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="15" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
         <v>41928037</v>
       </c>
@@ -788,8 +4059,11 @@
       <c r="K15" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O15" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="15" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
         <v>100237579</v>
       </c>
@@ -817,8 +4091,11 @@
       <c r="K16" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O16" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="15" x14ac:dyDescent="0.15">
       <c r="A17" s="3">
         <v>15332992</v>
       </c>
@@ -840,8 +4117,11 @@
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="3"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O17" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="15" x14ac:dyDescent="0.15">
       <c r="A18" s="3">
         <v>24990552</v>
       </c>
@@ -869,8 +4149,11 @@
       <c r="K18" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O18" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="15" x14ac:dyDescent="0.15">
       <c r="A19" s="3">
         <v>100202389</v>
       </c>
@@ -898,8 +4181,11 @@
       <c r="K19" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O19" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="15" x14ac:dyDescent="0.15">
       <c r="A20" s="3">
         <v>100305305</v>
       </c>
@@ -927,8 +4213,11 @@
       <c r="K20" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O20" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="15" x14ac:dyDescent="0.15">
       <c r="A21" s="3">
         <v>100260630</v>
       </c>
@@ -956,8 +4245,11 @@
       <c r="K21" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O21" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="15" x14ac:dyDescent="0.15">
       <c r="A22" s="3">
         <v>32437412</v>
       </c>
@@ -985,8 +4277,11 @@
       <c r="K22" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O22" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A23" s="3">
         <v>100373506</v>
       </c>
@@ -1015,7 +4310,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A24" s="3">
         <v>34560471</v>
       </c>
@@ -1044,7 +4339,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.15">
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
@@ -1058,7 +4353,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A26" s="3">
         <v>100832303</v>
       </c>
@@ -1087,7 +4382,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A27" s="3">
         <v>14348505</v>
       </c>
@@ -1116,7 +4411,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A28" s="3">
         <v>39636505</v>
       </c>
@@ -1145,7 +4440,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A29" s="3">
         <v>23419919</v>
       </c>
@@ -1174,7 +4469,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A30" s="3">
         <v>100673966</v>
       </c>
@@ -1203,7 +4498,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A31" s="3">
         <v>38339621</v>
       </c>
@@ -1232,7 +4527,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A32" s="3">
         <v>100765596</v>
       </c>
@@ -1261,7 +4556,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A33" s="3">
         <v>37535758</v>
       </c>
@@ -1290,7 +4585,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A34" s="3">
         <v>100486962</v>
       </c>
@@ -1319,7 +4614,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A35" s="3">
         <v>100291718</v>
       </c>
@@ -1348,7 +4643,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A36" s="3">
         <v>100876283</v>
       </c>
@@ -1377,7 +4672,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A37" s="3">
         <v>38619585</v>
       </c>
@@ -1406,7 +4701,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A38" s="3">
         <v>100186919</v>
       </c>
@@ -1435,7 +4730,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A39" s="3">
         <v>100166941</v>
       </c>
@@ -1464,7 +4759,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A40" s="3">
         <v>23033781</v>
       </c>
@@ -1493,7 +4788,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A41" s="3">
         <v>16946862</v>
       </c>
@@ -1522,7 +4817,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A42" s="3">
         <v>100347819</v>
       </c>
@@ -1551,7 +4846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A43" s="3">
         <v>41925437</v>
       </c>
@@ -1580,7 +4875,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A44" s="3">
         <v>16894321</v>
       </c>
@@ -1609,7 +4904,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A45" s="3">
         <v>100490151</v>
       </c>
@@ -1638,7 +4933,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A46" s="3">
         <v>32917707</v>
       </c>
@@ -1667,7 +4962,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A47" s="3">
         <v>40353379</v>
       </c>
@@ -1696,7 +4991,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A48" s="3">
         <v>100054442</v>
       </c>
@@ -1725,7 +5020,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A49" s="3">
         <v>100081485</v>
       </c>
@@ -1754,7 +5049,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A50" s="3">
         <v>24956684</v>
       </c>
@@ -1783,7 +5078,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A51" s="3">
         <v>19245524</v>
       </c>
@@ -1812,7 +5107,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A52" s="3">
         <v>100746009</v>
       </c>
@@ -1841,7 +5136,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A53" s="3">
         <v>41648946</v>
       </c>
@@ -1870,7 +5165,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A54" s="3">
         <v>41515235</v>
       </c>
@@ -1899,7 +5194,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A55" s="3">
         <v>13758645</v>
       </c>
@@ -1928,7 +5223,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A56" s="3">
         <v>32951624</v>
       </c>
@@ -1957,7 +5252,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A57" s="3">
         <v>36494463</v>
       </c>
@@ -1986,7 +5281,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A58" s="3">
         <v>100543977</v>
       </c>
@@ -2015,7 +5310,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A59" s="3">
         <v>100509202</v>
       </c>
@@ -2044,7 +5339,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A60" s="3">
         <v>100458631</v>
       </c>
@@ -2073,7 +5368,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A61" s="3">
         <v>27493518</v>
       </c>
@@ -2102,7 +5397,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A62" s="3">
         <v>32318423</v>
       </c>
@@ -2131,7 +5426,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A63" s="3">
         <v>21741358</v>
       </c>
@@ -2160,7 +5455,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A64" s="3">
         <v>23316468</v>
       </c>
@@ -2189,7 +5484,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A65" s="3">
         <v>100617086</v>
       </c>
@@ -2209,7 +5504,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A66" s="3">
         <v>100041859</v>
       </c>
@@ -2229,7 +5524,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A67" s="3">
         <v>41480661</v>
       </c>
@@ -2249,7 +5544,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A68" s="3">
         <v>36478834</v>
       </c>
@@ -2269,7 +5564,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A69" s="3">
         <v>27502593</v>
       </c>
@@ -2289,7 +5584,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A70" s="3">
         <v>100061317</v>
       </c>
@@ -2309,7 +5604,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A71" s="3">
         <v>36558994</v>
       </c>
@@ -2329,7 +5624,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A72" s="3">
         <v>100491624</v>
       </c>
@@ -2349,7 +5644,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A73" s="3">
         <v>100898699</v>
       </c>
@@ -2369,7 +5664,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A74" s="3">
         <v>35042088</v>
       </c>
@@ -2389,7 +5684,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A75" s="3">
         <v>100280479</v>
       </c>
@@ -2409,7 +5704,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A76" s="3">
         <v>28764571</v>
       </c>
@@ -2429,7 +5724,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A77" s="3">
         <v>100546896</v>
       </c>
@@ -2449,7 +5744,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A78" s="3">
         <v>100222157</v>
       </c>
@@ -2469,7 +5764,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A79" s="3">
         <v>35353914</v>
       </c>
@@ -2489,7 +5784,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A80" s="3">
         <v>100157550</v>
       </c>
@@ -2509,7 +5804,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A81" s="3">
         <v>30883184</v>
       </c>
@@ -2529,7 +5824,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A82" s="3">
         <v>34074801</v>
       </c>
@@ -2549,7 +5844,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A83" s="3">
         <v>100041018</v>
       </c>
@@ -2569,7 +5864,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A84" s="3">
         <v>39205427</v>
       </c>
@@ -2589,7 +5884,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A85" s="3">
         <v>100738919</v>
       </c>
@@ -2609,7 +5904,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A86" s="3">
         <v>100728540</v>
       </c>
@@ -2629,7 +5924,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A87" s="3">
         <v>40858453</v>
       </c>
@@ -2649,7 +5944,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A88" s="3">
         <v>100008638</v>
       </c>
@@ -2669,7 +5964,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A89" s="3">
         <v>100378248</v>
       </c>
@@ -2689,7 +5984,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A90" s="3">
         <v>28859922</v>
       </c>
@@ -2709,7 +6004,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A91" s="3">
         <v>100067667</v>
       </c>
@@ -2729,7 +6024,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A92" s="3">
         <v>100296221</v>
       </c>
@@ -2749,7 +6044,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A93" s="3">
         <v>25185638</v>
       </c>
@@ -2769,7 +6064,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A94" s="3">
         <v>101012485</v>
       </c>
@@ -2789,7 +6084,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A95" s="3">
         <v>100300947</v>
       </c>
@@ -2809,7 +6104,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.15">
       <c r="E96" s="3">
         <v>101012485</v>
       </c>
@@ -2820,7 +6115,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="5:7" x14ac:dyDescent="0.15">
       <c r="E97" s="3">
         <v>100300947</v>
       </c>

</xml_diff>

<commit_message>
updated likert plots without titles
</commit_message>
<xml_diff>
--- a/Oct Likert Numbers.xlsx
+++ b/Oct Likert Numbers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peterhiggins/Documents/RCode/elena_skin_uste/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F4D813B-7D50-7F49-8487-74C6DB01C8BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A69FB760-E529-1E4F-A3DC-1CB0A2822882}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21860" yWindow="1680" windowWidth="30580" windowHeight="27720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20620" yWindow="1080" windowWidth="30580" windowHeight="27720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="path" sheetId="3" r:id="rId1"/>
@@ -18,10 +18,19 @@
     <sheet name="imaging" sheetId="2" r:id="rId3"/>
     <sheet name="alt_format" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -3617,12 +3626,12 @@
   <dimension ref="A1:O97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T27" sqref="T27"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" customWidth="1"/>
+    <col min="1" max="1" width="17.83203125" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
     <col min="3" max="3" width="3.6640625" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>

</xml_diff>